<commit_message>
added mandatory fields check class
</commit_message>
<xml_diff>
--- a/target/classes/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
+++ b/target/classes/com/guru/qa/testdata/Guru99_NewCustomerCreationPage_FRAMEWORK.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16080" windowHeight="5955" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="NewCustomers" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="CustomerIdDataSheet" sheetId="4" r:id="rId4"/>
     <sheet name="AutoCompleteSampleSheet" sheetId="5" r:id="rId5"/>
     <sheet name="DataFromSeleniumEasyURL" sheetId="8" r:id="rId6"/>
+    <sheet name="DDDataFromSeleniumEasyURL" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
   <si>
     <t>Email</t>
   </si>
@@ -243,6 +244,24 @@
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
   </si>
 </sst>
 </file>
@@ -986,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1022,7 +1041,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,4 +1073,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>